<commit_message>
Se agregan nuevos archivos planos para pruebas con paises de menos datos, se modifica el archivo excel.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739B6087-4658-455B-8798-D9F6E7DA3B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B116FE7A-9231-4F01-B0DF-75068ED467E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Nombre de la Instancia</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>ILS (Iterated Local Search)</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
   </si>
 </sst>
 </file>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="122" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -655,147 +664,246 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>4663</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1">
-        <v>1290319</v>
+        <v>6656</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4">
-        <v>1646884</v>
+        <v>9745</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F6" si="0">(E4-C4)/E4</f>
-        <v>0.21650887372759708</v>
+        <v>0.31698306824012312</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3" t="e">
-        <f>(H4-C4)/H4</f>
-        <v>#DIV/0!</v>
+      <c r="H4" s="4">
+        <v>8106</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I6" si="1">(H4-C4)/H4</f>
+        <v>0.17887984209227734</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
       <c r="L4" s="3" t="e">
-        <f>(K4-F4)/K4</f>
+        <f t="shared" ref="L4:L6" si="2">(K4-F4)/K4</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>9882</v>
-      </c>
-      <c r="C5" s="2">
-        <v>300899</v>
+        <v>194</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9352</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="5">
-        <v>388944</v>
+      <c r="E5" s="4">
+        <v>11640</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>0.22636934880085566</v>
+        <v>0.19656357388316151</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="3" t="e">
-        <f>(H5-C5)/H5</f>
-        <v>#DIV/0!</v>
+      <c r="H5" s="4">
+        <v>11510</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.18748913987836663</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="3" t="e">
-        <f>(K5-F5)/K5</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>10639</v>
-      </c>
-      <c r="C6" s="2">
-        <v>520527</v>
+        <v>734</v>
+      </c>
+      <c r="C6" s="1">
+        <v>79114</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="5">
-        <v>649600</v>
+      <c r="E6" s="4">
+        <v>99247</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>0.19869612068965517</v>
+        <v>0.20285751710379155</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="3" t="e">
-        <f>(H6-C6)/H6</f>
-        <v>#DIV/0!</v>
+      <c r="H6" s="4">
+        <v>100147</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.2100212687349596</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="4"/>
       <c r="L6" s="3" t="e">
-        <f>(K6-F6)/K6</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="7">
-        <f>SUM(D3:D6)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <f>SUM(E3:E6)</f>
-        <v>2721816</v>
-      </c>
-      <c r="F7" s="8">
-        <f>AVERAGE(F3:F6)</f>
-        <v>0.22075002199228119</v>
-      </c>
-      <c r="G7" s="7">
-        <f>SUM(G3:G6)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <f>SUM(H3:H6)</f>
-        <v>30357</v>
-      </c>
-      <c r="I7" s="8" t="e">
-        <f>AVERAGE(I3:I6)</f>
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4663</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1290319</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4">
+        <v>1646884</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ref="F7:F9" si="3">(E7-C7)/E7</f>
+        <v>0.21650887372759708</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3" t="e">
+        <f>(H7-C7)/H7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="7">
-        <f>SUM(J3:J6)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <f>SUM(K3:K6)</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="8" t="e">
-        <f>AVERAGE(L3:L6)</f>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3" t="e">
+        <f>(K7-F7)/K7</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9882</v>
+      </c>
+      <c r="C8" s="2">
+        <v>300899</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="5">
+        <v>388944</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.22636934880085566</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="3" t="e">
+        <f>(H8-C8)/H8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3" t="e">
+        <f>(K8-F8)/K8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10639</v>
+      </c>
+      <c r="C9" s="2">
+        <v>520527</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5">
+        <v>649600</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.19869612068965517</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="3" t="e">
+        <f>(H9-C9)/H9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3" t="e">
+        <f>(K9-F9)/K9</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="7">
+        <f>SUM(D3:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <f>SUM(E3:E9)</f>
+        <v>2842448</v>
+      </c>
+      <c r="F10" s="8">
+        <f>AVERAGE(F3:F9)</f>
+        <v>0.22848632102802871</v>
+      </c>
+      <c r="G10" s="7">
+        <f>SUM(G3:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <f>SUM(H3:H9)</f>
+        <v>150120</v>
+      </c>
+      <c r="I10" s="8" t="e">
+        <f>AVERAGE(I3:I9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="7">
+        <f>SUM(J3:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <f>SUM(K3:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="8" t="e">
+        <f>AVERAGE(L3:L9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>

</xml_diff>

<commit_message>
se añaden los archivos para trabajar perturbacion, ILS y busqueda local. Además, se modifica el archivo de vencidario para trabajar el 2opt. La perturbación usa es la 3opt.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B116FE7A-9231-4F01-B0DF-75068ED467E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334843B2-F083-47CD-BF32-3D0DBAB213F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>JuanG</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{C9594333-4DFE-4F8F-8449-271BB4903745}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>JuanG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No toma en cuenta el tiempo que tarda en generar la matriz de distancias</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{E6E8D24C-A900-44DD-A0FC-EC29919F6ED4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>JuanG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No toma en cuenta el tiempo que tarda en generar la matriz de distancias</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
@@ -93,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +173,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -196,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +295,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,10 +627,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="122" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -572,35 +646,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
@@ -639,7 +713,9 @@
       <c r="C3" s="1">
         <v>27603</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="E3" s="4">
         <v>36388</v>
       </c>
@@ -647,7 +723,9 @@
         <f>(E3-C3)/E3</f>
         <v>0.24142574475101683</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H3" s="4">
         <v>30357</v>
       </c>
@@ -655,11 +733,15 @@
         <f>(H3-C3)/H3</f>
         <v>9.0720426919656094E-2</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="3" t="e">
-        <f>(K3-F3)/K3</f>
-        <v>#DIV/0!</v>
+      <c r="J3" s="2">
+        <v>2.5406</v>
+      </c>
+      <c r="K3" s="4">
+        <v>27603</v>
+      </c>
+      <c r="L3" s="3">
+        <f>(K3-C3)/K3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -672,7 +754,9 @@
       <c r="C4" s="1">
         <v>6656</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>8.0000000000000004E-4</v>
+      </c>
       <c r="E4" s="4">
         <v>9745</v>
       </c>
@@ -680,7 +764,9 @@
         <f t="shared" ref="F4:F6" si="0">(E4-C4)/E4</f>
         <v>0.31698306824012312</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>3.0999999999999999E-3</v>
+      </c>
       <c r="H4" s="4">
         <v>8106</v>
       </c>
@@ -688,11 +774,15 @@
         <f t="shared" ref="I4:I6" si="1">(H4-C4)/H4</f>
         <v>0.17887984209227734</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="3" t="e">
-        <f t="shared" ref="L4:L6" si="2">(K4-F4)/K4</f>
-        <v>#DIV/0!</v>
+      <c r="J4" s="10">
+        <v>4.8601999999999999</v>
+      </c>
+      <c r="K4" s="4">
+        <v>6808</v>
+      </c>
+      <c r="L4" s="3">
+        <f>(K4-C4)/K4</f>
+        <v>2.2326674500587545E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -705,7 +795,9 @@
       <c r="C5" s="1">
         <v>9352</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>4.3E-3</v>
+      </c>
       <c r="E5" s="4">
         <v>11640</v>
       </c>
@@ -713,7 +805,9 @@
         <f t="shared" si="0"/>
         <v>0.19656357388316151</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>0.1804</v>
+      </c>
       <c r="H5" s="4">
         <v>11510</v>
       </c>
@@ -721,11 +815,15 @@
         <f t="shared" si="1"/>
         <v>0.18748913987836663</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="J5" s="2">
+        <v>32.435699999999997</v>
+      </c>
+      <c r="K5" s="4">
+        <v>10830</v>
+      </c>
+      <c r="L5" s="3">
+        <f>(K5-C5)/K5</f>
+        <v>0.13647276084949214</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -738,7 +836,9 @@
       <c r="C6" s="1">
         <v>79114</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>5.3100000000000001E-2</v>
+      </c>
       <c r="E6" s="4">
         <v>99247</v>
       </c>
@@ -746,7 +846,9 @@
         <f t="shared" si="0"/>
         <v>0.20285751710379155</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>5.6135999999999999</v>
+      </c>
       <c r="H6" s="4">
         <v>100147</v>
       </c>
@@ -754,11 +856,15 @@
         <f t="shared" si="1"/>
         <v>0.2100212687349596</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="J6" s="2">
+        <v>79.882400000000004</v>
+      </c>
+      <c r="K6" s="4">
+        <v>95007</v>
+      </c>
+      <c r="L6" s="3">
+        <f>(K6-C6)/K6</f>
+        <v>0.16728241076973277</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -771,12 +877,14 @@
       <c r="C7" s="1">
         <v>1290319</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>4.3745000000000003</v>
+      </c>
       <c r="E7" s="4">
         <v>1646884</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F9" si="3">(E7-C7)/E7</f>
+        <f t="shared" ref="F7:F9" si="2">(E7-C7)/E7</f>
         <v>0.21650887372759708</v>
       </c>
       <c r="G7" s="2"/>
@@ -802,12 +910,14 @@
       <c r="C8" s="2">
         <v>300899</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>9.2074999999999996</v>
+      </c>
       <c r="E8" s="5">
         <v>388944</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.22636934880085566</v>
       </c>
       <c r="G8" s="2"/>
@@ -833,12 +943,14 @@
       <c r="C9" s="2">
         <v>520527</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>11.552</v>
+      </c>
       <c r="E9" s="5">
         <v>649600</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.19869612068965517</v>
       </c>
       <c r="G9" s="2"/>
@@ -855,14 +967,14 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="7">
         <f>SUM(D3:D9)</f>
-        <v>0</v>
+        <v>25.192399999999999</v>
       </c>
       <c r="E10" s="7">
         <f>SUM(E3:E9)</f>
@@ -874,7 +986,7 @@
       </c>
       <c r="G10" s="7">
         <f>SUM(G3:G9)</f>
-        <v>0</v>
+        <v>5.7984</v>
       </c>
       <c r="H10" s="7">
         <f>SUM(H3:H9)</f>
@@ -886,11 +998,11 @@
       </c>
       <c r="J10" s="7">
         <f>SUM(J3:J9)</f>
-        <v>0</v>
+        <v>119.7189</v>
       </c>
       <c r="K10" s="7">
         <f>SUM(K3:K9)</f>
-        <v>0</v>
+        <v>140248</v>
       </c>
       <c r="L10" s="8" t="e">
         <f>AVERAGE(L3:L9)</f>
@@ -911,10 +1023,20 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -923,15 +1045,6 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1130,20 +1243,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se agregan las graficas y se modifica el archivo excel para que corresponda con las nuevas ejecuciones y los valores de las gráficas.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334843B2-F083-47CD-BF32-3D0DBAB213F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB710C5-B9B8-466E-B4A0-01E01F8EDD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,7 @@
         <v>27603</v>
       </c>
       <c r="D3" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="4">
         <v>36388</v>
@@ -724,7 +724,7 @@
         <v>0.24142574475101683</v>
       </c>
       <c r="G3" s="2">
-        <v>1.2999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <v>30357</v>
@@ -734,7 +734,7 @@
         <v>9.0720426919656094E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>2.5406</v>
+        <v>1.9238</v>
       </c>
       <c r="K3" s="4">
         <v>27603</v>
@@ -755,7 +755,7 @@
         <v>6656</v>
       </c>
       <c r="D4" s="2">
-        <v>8.0000000000000004E-4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4">
         <v>9745</v>
@@ -765,7 +765,7 @@
         <v>0.31698306824012312</v>
       </c>
       <c r="G4" s="2">
-        <v>3.0999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H4" s="4">
         <v>8106</v>
@@ -778,11 +778,11 @@
         <v>4.8601999999999999</v>
       </c>
       <c r="K4" s="4">
-        <v>6808</v>
+        <v>7075</v>
       </c>
       <c r="L4" s="3">
         <f>(K4-C4)/K4</f>
-        <v>2.2326674500587545E-2</v>
+        <v>5.9222614840989396E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>9352</v>
       </c>
       <c r="D5" s="2">
-        <v>4.3E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E5" s="4">
         <v>11640</v>
@@ -806,7 +806,7 @@
         <v>0.19656357388316151</v>
       </c>
       <c r="G5" s="2">
-        <v>0.1804</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="H5" s="4">
         <v>11510</v>
@@ -816,14 +816,14 @@
         <v>0.18748913987836663</v>
       </c>
       <c r="J5" s="2">
-        <v>32.435699999999997</v>
+        <v>31.049299999999999</v>
       </c>
       <c r="K5" s="4">
-        <v>10830</v>
+        <v>10900</v>
       </c>
       <c r="L5" s="3">
         <f>(K5-C5)/K5</f>
-        <v>0.13647276084949214</v>
+        <v>0.14201834862385321</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>79114</v>
       </c>
       <c r="D6" s="2">
-        <v>5.3100000000000001E-2</v>
+        <v>3.4700000000000002E-2</v>
       </c>
       <c r="E6" s="4">
         <v>99247</v>
@@ -847,7 +847,7 @@
         <v>0.20285751710379155</v>
       </c>
       <c r="G6" s="2">
-        <v>5.6135999999999999</v>
+        <v>3.94</v>
       </c>
       <c r="H6" s="4">
         <v>100147</v>
@@ -857,14 +857,14 @@
         <v>0.2100212687349596</v>
       </c>
       <c r="J6" s="2">
-        <v>79.882400000000004</v>
+        <v>62.617800000000003</v>
       </c>
       <c r="K6" s="4">
-        <v>95007</v>
+        <v>95126</v>
       </c>
       <c r="L6" s="3">
         <f>(K6-C6)/K6</f>
-        <v>0.16728241076973277</v>
+        <v>0.16832411748628134</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -974,7 +974,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="7">
         <f>SUM(D3:D9)</f>
-        <v>25.192399999999999</v>
+        <v>25.171700000000001</v>
       </c>
       <c r="E10" s="7">
         <f>SUM(E3:E9)</f>
@@ -986,7 +986,7 @@
       </c>
       <c r="G10" s="7">
         <f>SUM(G3:G9)</f>
-        <v>5.7984</v>
+        <v>4.0171000000000001</v>
       </c>
       <c r="H10" s="7">
         <f>SUM(H3:H9)</f>
@@ -998,11 +998,11 @@
       </c>
       <c r="J10" s="7">
         <f>SUM(J3:J9)</f>
-        <v>119.7189</v>
+        <v>100.4511</v>
       </c>
       <c r="K10" s="7">
         <f>SUM(K3:K9)</f>
-        <v>140248</v>
+        <v>140704</v>
       </c>
       <c r="L10" s="8" t="e">
         <f>AVERAGE(L3:L9)</f>
@@ -1028,15 +1028,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1045,6 +1036,15 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1243,20 +1243,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se actualiza el archivo excel y el Readme.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB710C5-B9B8-466E-B4A0-01E01F8EDD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5637B-E0A6-42DE-B073-720789A1D344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1023,11 +1023,21 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1036,15 +1046,6 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1243,20 +1244,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Actualización del archivo FormatoPruebasRendimientoSegundoCorte.xlsx, reflejando cambios en los datos de rendimiento. Se revisan y ajustan las métricas para una mejor comparación de resultados en el contexto de las heurísticas implementadas.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5637B-E0A6-42DE-B073-720789A1D344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC18D767-611B-40F1-9E0A-4A18805B5366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Nombre de la Instancia</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Genético (Chu-Beasley)</t>
   </si>
 </sst>
 </file>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -643,9 +646,10 @@
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -670,8 +674,13 @@
       </c>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
+      <c r="M1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -702,8 +711,17 @@
       <c r="L2" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="M2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -724,7 +742,7 @@
         <v>0.24142574475101683</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H3" s="4">
         <v>30357</v>
@@ -734,17 +752,27 @@
         <v>9.0720426919656094E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>1.9238</v>
+        <v>2.8788999999999998</v>
       </c>
       <c r="K3" s="4">
-        <v>27603</v>
+        <v>27750</v>
       </c>
       <c r="L3" s="3">
         <f>(K3-C3)/K3</f>
-        <v>0</v>
+        <v>5.2972972972972973E-3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.3024</v>
+      </c>
+      <c r="N3" s="4">
+        <v>28138</v>
+      </c>
+      <c r="O3" s="3">
+        <f>(N3-C3)/N3</f>
+        <v>1.9013433790603454E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -765,7 +793,7 @@
         <v>0.31698306824012312</v>
       </c>
       <c r="G4" s="2">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="H4" s="4">
         <v>8106</v>
@@ -775,17 +803,27 @@
         <v>0.17887984209227734</v>
       </c>
       <c r="J4" s="10">
-        <v>4.8601999999999999</v>
+        <v>11.7013</v>
       </c>
       <c r="K4" s="4">
-        <v>7075</v>
+        <v>6656</v>
       </c>
       <c r="L4" s="3">
         <f>(K4-C4)/K4</f>
-        <v>5.9222614840989396E-2</v>
+        <v>0</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6656</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" ref="O4:O9" si="2">(N4-C4)/N4</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -796,7 +834,7 @@
         <v>9352</v>
       </c>
       <c r="D5" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E5" s="4">
         <v>11640</v>
@@ -806,7 +844,7 @@
         <v>0.19656357388316151</v>
       </c>
       <c r="G5" s="2">
-        <v>7.6100000000000001E-2</v>
+        <v>7.3099999999999998E-2</v>
       </c>
       <c r="H5" s="4">
         <v>11510</v>
@@ -816,17 +854,27 @@
         <v>0.18748913987836663</v>
       </c>
       <c r="J5" s="2">
-        <v>31.049299999999999</v>
+        <v>62.494700000000002</v>
       </c>
       <c r="K5" s="4">
-        <v>10900</v>
+        <v>10743</v>
       </c>
       <c r="L5" s="3">
         <f>(K5-C5)/K5</f>
-        <v>0.14201834862385321</v>
+        <v>0.12947966117471843</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4.9939</v>
+      </c>
+      <c r="N5" s="4">
+        <v>9972</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="2"/>
+        <v>6.2174087444845566E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -837,7 +885,7 @@
         <v>79114</v>
       </c>
       <c r="D6" s="2">
-        <v>3.4700000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E6" s="4">
         <v>99247</v>
@@ -847,7 +895,7 @@
         <v>0.20285751710379155</v>
       </c>
       <c r="G6" s="2">
-        <v>3.94</v>
+        <v>3.7833000000000001</v>
       </c>
       <c r="H6" s="4">
         <v>100147</v>
@@ -857,17 +905,27 @@
         <v>0.2100212687349596</v>
       </c>
       <c r="J6" s="2">
-        <v>62.617800000000003</v>
+        <v>77.623099999999994</v>
       </c>
       <c r="K6" s="4">
-        <v>95126</v>
+        <v>95237</v>
       </c>
       <c r="L6" s="3">
         <f>(K6-C6)/K6</f>
-        <v>0.16832411748628134</v>
+        <v>0.16929344687463907</v>
+      </c>
+      <c r="M6" s="2">
+        <v>234.54519999999999</v>
+      </c>
+      <c r="N6" s="4">
+        <v>87238</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="2"/>
+        <v>9.3124555812833854E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -884,7 +942,7 @@
         <v>1646884</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F9" si="2">(E7-C7)/E7</f>
+        <f t="shared" ref="F7:F9" si="3">(E7-C7)/E7</f>
         <v>0.21650887372759708</v>
       </c>
       <c r="G7" s="2"/>
@@ -899,8 +957,14 @@
         <f>(K7-F7)/K7</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -917,7 +981,7 @@
         <v>388944</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.22636934880085566</v>
       </c>
       <c r="G8" s="2"/>
@@ -932,8 +996,14 @@
         <f>(K8-F8)/K8</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -950,7 +1020,7 @@
         <v>649600</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.19869612068965517</v>
       </c>
       <c r="G9" s="2"/>
@@ -965,8 +1035,14 @@
         <f>(K9-F9)/K9</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
@@ -974,7 +1050,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="7">
         <f>SUM(D3:D9)</f>
-        <v>25.171700000000001</v>
+        <v>25.169999999999998</v>
       </c>
       <c r="E10" s="7">
         <f>SUM(E3:E9)</f>
@@ -986,7 +1062,7 @@
       </c>
       <c r="G10" s="7">
         <f>SUM(G3:G9)</f>
-        <v>4.0171000000000001</v>
+        <v>3.8593999999999999</v>
       </c>
       <c r="H10" s="7">
         <f>SUM(H3:H9)</f>
@@ -998,22 +1074,35 @@
       </c>
       <c r="J10" s="7">
         <f>SUM(J3:J9)</f>
-        <v>100.4511</v>
+        <v>154.69799999999998</v>
       </c>
       <c r="K10" s="7">
         <f>SUM(K3:K9)</f>
-        <v>140704</v>
+        <v>140386</v>
       </c>
       <c r="L10" s="8" t="e">
         <f>AVERAGE(L3:L9)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="M10" s="7">
+        <f>SUM(M3:M9)</f>
+        <v>240.1437</v>
+      </c>
+      <c r="N10" s="7">
+        <f>SUM(N3:N9)</f>
+        <v>132004</v>
+      </c>
+      <c r="O10" s="8" t="e">
+        <f>AVERAGE(O3:O9)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A1:A2"/>
@@ -1029,15 +1118,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1046,6 +1126,15 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1244,20 +1333,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Optimización del método de cruce PMX en el algoritmo genético. Se mejora la gestión de duplicados y se implementa una verificación final para asegurar la validez del tour generado. Se actualizan gráficos de rendimiento y se corrigen archivos binarios relacionados.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC18D767-611B-40F1-9E0A-4A18805B5366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F875774C-5BAD-4C77-B48A-8B9072DD5BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -634,7 +634,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -915,14 +915,14 @@
         <v>0.16929344687463907</v>
       </c>
       <c r="M6" s="2">
-        <v>234.54519999999999</v>
+        <v>412.65530000000001</v>
       </c>
       <c r="N6" s="4">
-        <v>87238</v>
+        <v>87091</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" si="2"/>
-        <v>9.3124555812833854E-2</v>
+        <v>9.1593850110803648E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1086,11 +1086,11 @@
       </c>
       <c r="M10" s="7">
         <f>SUM(M3:M9)</f>
-        <v>240.1437</v>
+        <v>418.25380000000001</v>
       </c>
       <c r="N10" s="7">
         <f>SUM(N3:N9)</f>
-        <v>132004</v>
+        <v>131857</v>
       </c>
       <c r="O10" s="8" t="e">
         <f>AVERAGE(O3:O9)</f>
@@ -1118,6 +1118,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1126,15 +1135,6 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,20 +1333,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se añade validación de archivos TSP en el script principal, mejorando la gestión de errores y la experiencia del usuario. Se implementa un menú principal que permite ejecutar algoritmos directamente con un archivo especificado como argumento. Se eliminan funciones obsoletas relacionadas con la selección de datasets. Se actualiza el archivo de ayuda para reflejar los nuevos cambios en la ejecución del programa.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F875774C-5BAD-4C77-B48A-8B9072DD5BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E803E4-3A26-4038-A464-76085287E4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1118,15 +1118,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1135,6 +1126,15 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,20 +1333,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se añade la funcionalidad para ejecutar el algoritmo TSP utilizando OR-Tools, incluyendo la generación de gráficas comparativas de resultados entre diferentes metaheurísticas. Se actualiza el menú principal para incluir esta nueva opción y se implementa la gestión de errores y visualización de resultados. Además, se actualiza el archivo FormatoPruebasRendimientoSegundoCorte.xlsx para reflejar los cambios en los datos de rendimiento.
</commit_message>
<xml_diff>
--- a/FormatoPruebasRendimientoSegundoCorte.xlsx
+++ b/FormatoPruebasRendimientoSegundoCorte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanG\Documents\salesman-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E803E4-3A26-4038-A464-76085287E4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75645E1B-B928-4675-A13E-82DF43A3370A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBFDDC12-32D8-8040-A9BB-2AB090F1F042}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Nombre de la Instancia</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Genético (Chu-Beasley)</t>
+  </si>
+  <si>
+    <t>TSP ORTools</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83ACD2-5CC7-664F-A4E0-3B79117716F4}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -649,7 +652,7 @@
     <col min="14" max="14" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -679,8 +682,13 @@
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -720,8 +728,17 @@
       <c r="O2" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="P2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -771,8 +788,18 @@
         <f>(N3-C3)/N3</f>
         <v>1.9013433790603454E-2</v>
       </c>
+      <c r="P3" s="2">
+        <v>10.0016</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>27603</v>
+      </c>
+      <c r="R3" s="3">
+        <f>(Q3-C3)/Q3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -822,8 +849,18 @@
         <f t="shared" ref="O4:O9" si="2">(N4-C4)/N4</f>
         <v>0</v>
       </c>
+      <c r="P4" s="10">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>6656</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" ref="R4:R6" si="3">(Q4-C4)/Q4</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -870,11 +907,21 @@
         <v>9972</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="2"/>
+        <f>(N5-C5)/N5</f>
         <v>6.2174087444845566E-2</v>
       </c>
+      <c r="P5" s="2">
+        <v>10.001799999999999</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>9755</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" si="3"/>
+        <v>4.131214761660687E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -924,8 +971,18 @@
         <f t="shared" si="2"/>
         <v>9.1593850110803648E-2</v>
       </c>
+      <c r="P6" s="2">
+        <v>10.017899999999999</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>85724</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" si="3"/>
+        <v>7.7107927768186271E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -942,7 +999,7 @@
         <v>1646884</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F9" si="3">(E7-C7)/E7</f>
+        <f t="shared" ref="F7:F9" si="4">(E7-C7)/E7</f>
         <v>0.21650887372759708</v>
       </c>
       <c r="G7" s="2"/>
@@ -963,8 +1020,14 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="3" t="e">
+        <f t="shared" ref="R4:R9" si="5">(Q7-F7)/Q7</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -981,7 +1044,7 @@
         <v>388944</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22636934880085566</v>
       </c>
       <c r="G8" s="2"/>
@@ -1002,8 +1065,14 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1089,7 @@
         <v>649600</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19869612068965517</v>
       </c>
       <c r="G9" s="2"/>
@@ -1041,8 +1110,14 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
@@ -1096,12 +1171,25 @@
         <f>AVERAGE(O3:O9)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="P10" s="7">
+        <f>SUM(P3:P9)</f>
+        <v>30.072699999999998</v>
+      </c>
+      <c r="Q10" s="7">
+        <f>SUM(Q3:Q9)</f>
+        <v>129738</v>
+      </c>
+      <c r="R10" s="8" t="e">
+        <f>AVERAGE(R3:R9)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="A10:C10"/>
@@ -1118,6 +1206,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b57cc97-55ee-4b28-87ae-29d56e21bbf9">
@@ -1126,15 +1223,6 @@
     <TaxCatchAll xmlns="db919950-9ade-4ed0-af76-99c05809cac8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,20 +1421,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B8ABE5F-2D3C-4A44-A543-814B1FA70DC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2b57cc97-55ee-4b28-87ae-29d56e21bbf9"/>
     <ds:schemaRef ds:uri="db919950-9ade-4ed0-af76-99c05809cac8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B377D5C-C6E8-43B4-9005-EE40747FBCE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>